<commit_message>
Add UI translation capabilities
</commit_message>
<xml_diff>
--- a/i18n/pt.xlsx
+++ b/i18n/pt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matej\Programming\wingsearch\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="13_ncr:1_{901EC647-1EE6-4D6B-921A-383110F343FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5FB7CAE-4249-4272-9D65-0B40A1AE7FD9}"/>
+  <xr:revisionPtr revIDLastSave="571" documentId="13_ncr:1_{901EC647-1EE6-4D6B-921A-383110F343FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A7DF7C3-62C7-490F-9554-197318F4C381}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2798" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2871" uniqueCount="1031">
   <si>
     <t>id</t>
   </si>
@@ -2884,40 +2884,256 @@
     <t>Translated</t>
   </si>
   <si>
+    <t>card.whenActivated</t>
+  </si>
+  <si>
     <t>WHEN ACTIVATED</t>
   </si>
   <si>
     <t>QUANDO ATIVADO</t>
   </si>
   <si>
+    <t>card.whenPlayed</t>
+  </si>
+  <si>
     <t>WHEN PLAYED</t>
   </si>
   <si>
     <t>QUANDO JOGADO</t>
   </si>
   <si>
+    <t>card.betweenTurns</t>
+  </si>
+  <si>
     <t>ONCE BETWEEN TURNS</t>
   </si>
   <si>
     <t>UMA VEZ ENTRE TURNOS</t>
   </si>
   <si>
+    <t>card.roundEnd</t>
+  </si>
+  <si>
     <t>ROUND END</t>
   </si>
   <si>
     <t>FINAL DE RODADA</t>
   </si>
   <si>
+    <t>card.gameEnd</t>
+  </si>
+  <si>
     <t>GAME END</t>
   </si>
   <si>
     <t>FIM DE JOGO</t>
   </si>
   <si>
+    <t>card.ofCards</t>
+  </si>
+  <si>
     <t>of cards</t>
   </si>
   <si>
     <t>de cartas</t>
+  </si>
+  <si>
+    <t>search.label.cardName</t>
+  </si>
+  <si>
+    <t>Search birds and bonus cards</t>
+  </si>
+  <si>
+    <t>Pesquisar aves e cartas bônus</t>
+  </si>
+  <si>
+    <t>search.hint.cardName</t>
+  </si>
+  <si>
+    <t>Use card name or description</t>
+  </si>
+  <si>
+    <t>Utilize o nome da carta ou descrição</t>
+  </si>
+  <si>
+    <t>search.label.bonusCard</t>
+  </si>
+  <si>
+    <t>Search birds by applicable bonus cards</t>
+  </si>
+  <si>
+    <t>Pesquisar aves por carta bônus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search.hint.bonusCard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use bonus card name or condition </t>
+  </si>
+  <si>
+    <t>Utilize o nome da carta bônus ou condição</t>
+  </si>
+  <si>
+    <t>search.tooltip.powerType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle birds with a specific power color </t>
+  </si>
+  <si>
+    <t>Mostrar aves com a cor de poder específica</t>
+  </si>
+  <si>
+    <t>search.tooltip.foodType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle birds with a specific food cost </t>
+  </si>
+  <si>
+    <t>Mostrar aves com o custo de comida específico</t>
+  </si>
+  <si>
+    <t>search.tooltip.nestType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle birds with a specific nest type </t>
+  </si>
+  <si>
+    <t>Mostrar aves com o tipo de ninho específico</t>
+  </si>
+  <si>
+    <t>search.tooltip.eggCapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by the egg capacity </t>
+  </si>
+  <si>
+    <t>Filtrar por capacidade de ovos</t>
+  </si>
+  <si>
+    <t>search.tooltip.pointsNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by the number of points </t>
+  </si>
+  <si>
+    <t>Filtrar pelo número de pontos</t>
+  </si>
+  <si>
+    <t>search.tooltip.wingspan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by wingspan </t>
+  </si>
+  <si>
+    <t>Filtrar por envergadura</t>
+  </si>
+  <si>
+    <t>search.tooltip.foodCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by food cost </t>
+  </si>
+  <si>
+    <t>Filtrar por custo de comida</t>
+  </si>
+  <si>
+    <t>search.tooltip.beakType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle birds with a specific beak type </t>
+  </si>
+  <si>
+    <t>Mostrar aves com um tipo específico de bico</t>
+  </si>
+  <si>
+    <t>search.tooltip.filterBonuses</t>
+  </si>
+  <si>
+    <t>Filter out all bonuses</t>
+  </si>
+  <si>
+    <t>Ocultar todos os bônus</t>
+  </si>
+  <si>
+    <t>search.tooltip.countBonuses</t>
+  </si>
+  <si>
+    <t>Count in all bonuses</t>
+  </si>
+  <si>
+    <t>Considerar todos os bônus</t>
+  </si>
+  <si>
+    <t>search.tooltip.filterBirds</t>
+  </si>
+  <si>
+    <t>Filter out all birds</t>
+  </si>
+  <si>
+    <t>Ocultar todas as aves</t>
+  </si>
+  <si>
+    <t>search.tooltip.countBirds</t>
+  </si>
+  <si>
+    <t>Count in all birds</t>
+  </si>
+  <si>
+    <t>Considerar todas as aves</t>
+  </si>
+  <si>
+    <t>search.tooltip.habitatType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter birds that can live in a specific habitat </t>
+  </si>
+  <si>
+    <t>Mostrar aves que podem viver em um determinado habitat</t>
+  </si>
+  <si>
+    <t>search.tooltip.resetFilters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset all filters (except expansions) </t>
+  </si>
+  <si>
+    <t>Limpar todos os filtros (exceto expansões)</t>
+  </si>
+  <si>
+    <t>search.button.reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset </t>
+  </si>
+  <si>
+    <t>Limpar</t>
+  </si>
+  <si>
+    <t>search.tooltip.languageMoreInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More about language support </t>
+  </si>
+  <si>
+    <t>Mais informações sobre o suporte de idiomas</t>
+  </si>
+  <si>
+    <t>search.label.language</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>search.label.expansions</t>
+  </si>
+  <si>
+    <t>Expansions</t>
+  </si>
+  <si>
+    <t>Expansões</t>
   </si>
 </sst>
 </file>
@@ -3070,9 +3286,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AA05F43-7971-4EB4-8E5C-9E7EFB591048}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{A5CFAA4D-6579-4D29-89EB-6C57AE6E1FEB}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AA05F43-7971-4EB4-8E5C-9E7EFB591048}" name="Table4" displayName="Table4" ref="A1:C29" totalsRowShown="0">
+  <autoFilter ref="A1:C29" xr:uid="{A5CFAA4D-6579-4D29-89EB-6C57AE6E1FEB}"/>
+  <tableColumns count="3">
+    <tableColumn id="3" xr3:uid="{EF0477AE-ED4C-4BD5-BCBF-867F67AADF36}" name="id"/>
     <tableColumn id="1" xr3:uid="{EA688C91-7F6D-4D7A-9D79-A30EB35759F6}" name="English name"/>
     <tableColumn id="2" xr3:uid="{3A0CACDB-DCE4-4775-8258-271B6485FC6A}" name="Translated"/>
   </tableColumns>
@@ -13032,7 +13249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F73C7-BAF7-4DDB-A3F3-74A889132A9F}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -13804,72 +14021,336 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D758ED0-344A-47B5-8000-C5BBB7F38038}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>947</v>
       </c>
       <c r="B2" t="s">
         <v>948</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B3" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>951</v>
+      </c>
+      <c r="C3" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B4" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>954</v>
+      </c>
+      <c r="C4" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="B5" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>957</v>
+      </c>
+      <c r="C5" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="B6" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>960</v>
+      </c>
+      <c r="C6" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>957</v>
+        <v>962</v>
       </c>
       <c r="B7" t="s">
-        <v>958</v>
+        <v>963</v>
+      </c>
+      <c r="C7" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1">
+      <c r="A8" t="s">
+        <v>965</v>
+      </c>
+      <c r="B8" t="s">
+        <v>966</v>
+      </c>
+      <c r="C8" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1">
+      <c r="A9" t="s">
+        <v>968</v>
+      </c>
+      <c r="B9" t="s">
+        <v>969</v>
+      </c>
+      <c r="C9" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1">
+      <c r="A10" t="s">
+        <v>971</v>
+      </c>
+      <c r="B10" t="s">
+        <v>972</v>
+      </c>
+      <c r="C10" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1">
+      <c r="A11" t="s">
+        <v>974</v>
+      </c>
+      <c r="B11" t="s">
+        <v>975</v>
+      </c>
+      <c r="C11" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1">
+      <c r="A12" t="s">
+        <v>977</v>
+      </c>
+      <c r="B12" t="s">
+        <v>978</v>
+      </c>
+      <c r="C12" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="A13" t="s">
+        <v>980</v>
+      </c>
+      <c r="B13" t="s">
+        <v>981</v>
+      </c>
+      <c r="C13" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1">
+      <c r="A14" t="s">
+        <v>983</v>
+      </c>
+      <c r="B14" t="s">
+        <v>984</v>
+      </c>
+      <c r="C14" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1">
+      <c r="A15" t="s">
+        <v>986</v>
+      </c>
+      <c r="B15" t="s">
+        <v>987</v>
+      </c>
+      <c r="C15" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1">
+      <c r="A16" t="s">
+        <v>989</v>
+      </c>
+      <c r="B16" t="s">
+        <v>990</v>
+      </c>
+      <c r="C16" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1">
+      <c r="A17" t="s">
+        <v>992</v>
+      </c>
+      <c r="B17" t="s">
+        <v>993</v>
+      </c>
+      <c r="C17" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1">
+      <c r="A18" t="s">
+        <v>995</v>
+      </c>
+      <c r="B18" t="s">
+        <v>996</v>
+      </c>
+      <c r="C18" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1">
+      <c r="A19" t="s">
+        <v>998</v>
+      </c>
+      <c r="B19" t="s">
+        <v>999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1">
+      <c r="A20" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1">
+      <c r="A21" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1">
+      <c r="A22" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1">
+      <c r="A24" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1">
+      <c r="A25" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1">
+      <c r="A26" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1">
+      <c r="A27" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1">
+      <c r="A28" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1">
+      <c r="A29" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>